<commit_message>
FINISHED SQA SIGNOFF FACULTY
I ALSO FIXED A DEFECT REGARDING EMAIL ADDRESS BEING LOWER-CASE. MODIFIED
SOME OF MY FACULTY TEST FILES.
</commit_message>
<xml_diff>
--- a/TestFiles/Test files for facultyMembers/FileIndex.xlsx
+++ b/TestFiles/Test files for facultyMembers/FileIndex.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="9555" windowHeight="7740"/>
+    <workbookView xWindow="360" yWindow="165" windowWidth="9555" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,9 +30,6 @@
     <t>No space after comma that follows the last name of the faculty member. The input is rejected.</t>
   </si>
   <si>
-    <t>Input rejected. Less than 3 hours.</t>
-  </si>
-  <si>
     <t>Input rejected. Years of service exceeds the maxiumum of  60.</t>
   </si>
   <si>
@@ -123,24 +120,12 @@
     <t>Input rejected. Empty file.</t>
   </si>
   <si>
-    <t>Input rejected. Years of service is less than zero</t>
-  </si>
-  <si>
     <t>Input rejected. First name of faculty is not all upper-case.</t>
   </si>
   <si>
-    <t>Input rejected. Decimal numbers are not acceptable.</t>
-  </si>
-  <si>
     <t>Input rejected. Years of service cannot be a decimal number.</t>
   </si>
   <si>
-    <t>Input rejected. Email length exceeds the maximum of 10.</t>
-  </si>
-  <si>
-    <t>Input is rejected. Email length is less than the minimum 3.</t>
-  </si>
-  <si>
     <t>Input should be accepted. The minimum hours teaching is three.</t>
   </si>
   <si>
@@ -150,12 +135,6 @@
     <t>Input should be accepted. Large amount of input.</t>
   </si>
   <si>
-    <t>The input is not accepted. No space follows the comma in faculty name. No space between  the last name and year of service, and the hours teaching is less than the minimum.</t>
-  </si>
-  <si>
-    <t>Input is not accepted because the last name is lower-case, the years of service is greater than the maximum of 60. The email address is all lowercase.</t>
-  </si>
-  <si>
     <t>Input is not accepted because the "@UNA.EDU" is missing from email. The name has the number "12" preceeding it.</t>
   </si>
   <si>
@@ -172,6 +151,27 @@
   </si>
   <si>
     <t>The first line in the input file is missing the years of service. The second line in the input file has the same email address for a different faulty member.</t>
+  </si>
+  <si>
+    <t>Line one input rejected minimum teaching hours is 1.</t>
+  </si>
+  <si>
+    <t>Line 1 input rejected. Decimal numbers are not acceptable.</t>
+  </si>
+  <si>
+    <t>Line one input rejected because email extension is partially lowercase</t>
+  </si>
+  <si>
+    <t>Line one input rejected. Email length exceeds the maximum of 10.</t>
+  </si>
+  <si>
+    <t>line one input is rejected. Email length is less than the minimum 3.</t>
+  </si>
+  <si>
+    <t>All file input is not accepted. Line 1 minimum hours is less than three. Line two email extension is partially lower-case. Line three email address is lower-case. Line four only part of email address is lower-case.</t>
+  </si>
+  <si>
+    <t>File contents not accepted. Line one last name is lower-case. Line two first name is lower-case, and line three is missing a space between last and first name.</t>
   </si>
 </sst>
 </file>
@@ -560,8 +560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -581,23 +581,23 @@
     </row>
     <row r="2" spans="1:2" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>3</v>
@@ -605,7 +605,7 @@
     </row>
     <row r="5" spans="1:2" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>2</v>
@@ -613,170 +613,170 @@
     </row>
     <row r="6" spans="1:2" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="B22" s="2" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="87" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>